<commit_message>
Funciones de filtracion terminada
</commit_message>
<xml_diff>
--- a/src/helpers/reports/Empresas.xlsx
+++ b/src/helpers/reports/Empresas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -37,7 +37,7 @@
     <t>"67be9ec5ef685590dc9b7fe1"</t>
   </si>
   <si>
-    <t>Universidad Mariano Galvez de Guatemala</t>
+    <t>UMG</t>
   </si>
   <si>
     <t>ALTO</t>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Distribuidora</t>
+  </si>
+  <si>
+    <t>"67c1adb6a7cf6af9db40f795"</t>
+  </si>
+  <si>
+    <t>HyperX</t>
+  </si>
+  <si>
+    <t>Joaquin Figueroa, Saul de Leon</t>
   </si>
 </sst>
 </file>
@@ -474,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -647,6 +656,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>